<commit_message>
Assets + test trash + modif Grid + Icon
</commit_message>
<xml_diff>
--- a/Assets/Data/Weights.xlsx
+++ b/Assets/Data/Weights.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21620" windowHeight="13480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21620" windowHeight="13480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Poids" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="Weights.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:francoisezitouni:Documents:MPTangam:Assets:Data:Weights.txt" decimal="," thousands=" " delimiter=":">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:francoisezitouni:Documents:MPTangam:Assets:Data:Weights.txt" decimal="," thousands=" " delimiter=":">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -171,9 +171,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -219,7 +235,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="52">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="6" builtinId="8" hidden="1"/>
@@ -237,6 +253,14 @@
     <cellStyle name="Lien hypertexte" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
@@ -254,6 +278,14 @@
     <cellStyle name="Lien hypertexte visité" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -588,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="D2:F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="A20:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -653,19 +685,19 @@
         <v>2</v>
       </c>
       <c r="G2" s="2">
-        <f>C2/SUM(C:C)</f>
+        <f t="shared" ref="G2:G19" si="0">C2/SUM(C:C)</f>
         <v>0</v>
       </c>
       <c r="H2" s="2">
-        <f>D2/SUM(D:D)</f>
+        <f t="shared" ref="H2:H19" si="1">D2/SUM(D:D)</f>
         <v>0.1</v>
       </c>
       <c r="I2" s="2">
-        <f>E2/SUM(E:E)</f>
+        <f t="shared" ref="I2:I19" si="2">E2/SUM(E:E)</f>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J2" s="2">
-        <f>F2/SUM(F:F)</f>
+        <f t="shared" ref="J2:J19" si="3">F2/SUM(F:F)</f>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -689,19 +721,19 @@
         <v>2</v>
       </c>
       <c r="G3" s="2">
-        <f>C3/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H3" s="2">
-        <f>D3/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I3" s="2">
-        <f>E3/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J3" s="2">
-        <f>F3/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -725,19 +757,19 @@
         <v>2</v>
       </c>
       <c r="G4" s="2">
-        <f>C4/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <f>D4/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I4" s="2">
-        <f>E4/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J4" s="2">
-        <f>F4/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -761,19 +793,19 @@
         <v>2</v>
       </c>
       <c r="G5" s="2">
-        <f>C5/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5" s="2">
-        <f>D5/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I5" s="2">
-        <f>E5/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J5" s="2">
-        <f>F5/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -797,19 +829,19 @@
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <f>C6/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6" s="2">
-        <f>D6/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f>E6/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J6" s="2">
-        <f>F6/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>2.8571428571428571E-2</v>
       </c>
     </row>
@@ -833,19 +865,19 @@
         <v>1</v>
       </c>
       <c r="G7" s="2">
-        <f>C7/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" s="2">
-        <f>D7/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <f>E7/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J7" s="2">
-        <f>F7/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>2.8571428571428571E-2</v>
       </c>
     </row>
@@ -869,19 +901,19 @@
         <v>1</v>
       </c>
       <c r="G8" s="2">
-        <f>C8/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8" s="2">
-        <f>D8/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I8" s="2">
-        <f>E8/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J8" s="2">
-        <f>F8/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>2.8571428571428571E-2</v>
       </c>
     </row>
@@ -905,19 +937,19 @@
         <v>1</v>
       </c>
       <c r="G9" s="2">
-        <f>C9/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" s="2">
-        <f>D9/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <f>E9/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J9" s="2">
-        <f>F9/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>2.8571428571428571E-2</v>
       </c>
     </row>
@@ -941,19 +973,19 @@
         <v>2</v>
       </c>
       <c r="G10" s="2">
-        <f>C10/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <f>D10/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10" s="2">
-        <f>E10/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J10" s="2">
-        <f>F10/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -977,19 +1009,19 @@
         <v>2</v>
       </c>
       <c r="G11" s="2">
-        <f>C11/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" s="2">
-        <f>D11/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I11" s="2">
-        <f>E11/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J11" s="2">
-        <f>F11/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -1013,19 +1045,19 @@
         <v>2</v>
       </c>
       <c r="G12" s="2">
-        <f>C12/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="2">
-        <f>D12/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I12" s="2">
-        <f>E12/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J12" s="2">
-        <f>F12/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -1049,19 +1081,19 @@
         <v>2</v>
       </c>
       <c r="G13" s="2">
-        <f>C13/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="2">
-        <f>D13/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I13" s="2">
-        <f>E13/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J13" s="2">
-        <f>F13/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -1082,19 +1114,19 @@
         <v>2</v>
       </c>
       <c r="G14" s="2">
-        <f>C14/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="2">
-        <f>D14/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I14" s="2">
-        <f>E14/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J14" s="2">
-        <f>F14/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -1115,19 +1147,19 @@
         <v>1</v>
       </c>
       <c r="G15" s="2">
-        <f>C15/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="2">
-        <f>D15/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I15" s="2">
-        <f>E15/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J15" s="2">
-        <f>F15/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>2.8571428571428571E-2</v>
       </c>
     </row>
@@ -1151,19 +1183,19 @@
         <v>2</v>
       </c>
       <c r="G16" s="2">
-        <f>C16/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="H16" s="2">
-        <f>D16/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I16" s="2">
-        <f>E16/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J16" s="2">
-        <f>F16/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -1187,19 +1219,19 @@
         <v>2</v>
       </c>
       <c r="G17" s="2">
-        <f>C17/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="H17" s="2">
-        <f>D17/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I17" s="2">
-        <f>E17/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J17" s="2">
-        <f>F17/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -1223,19 +1255,19 @@
         <v>2</v>
       </c>
       <c r="G18" s="2">
-        <f>C18/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="H18" s="2">
-        <f>D18/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I18" s="2">
-        <f>E18/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J18" s="2">
-        <f>F18/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
@@ -1259,24 +1291,48 @@
         <v>2</v>
       </c>
       <c r="G19" s="2">
-        <f>C19/SUM(C:C)</f>
+        <f t="shared" si="0"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="H19" s="2">
-        <f>D19/SUM(D:D)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I19" s="2">
-        <f>E19/SUM(E:E)</f>
+        <f t="shared" si="2"/>
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="J19" s="2">
-        <f>F19/SUM(F:F)</f>
+        <f t="shared" si="3"/>
         <v>5.7142857142857141E-2</v>
       </c>
     </row>
+    <row r="20" spans="1:10">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1290,7 +1346,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -1304,7 +1360,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -1318,7 +1374,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J19">
+  <conditionalFormatting sqref="J2:J23">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -1346,7 +1402,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G2:G19</xm:sqref>
+          <xm:sqref>G2:G23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5C243F4B-53B6-1341-A631-F4DCCA06D945}">
@@ -1357,7 +1413,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H2:H19</xm:sqref>
+          <xm:sqref>H2:H23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6CAA247C-236A-9F4F-AF4E-A477F2A4A83F}">
@@ -1368,7 +1424,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I2:I19</xm:sqref>
+          <xm:sqref>I2:I23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1A1D8572-22C2-154A-A5E5-19616B3CB2D2}">
@@ -1379,7 +1435,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J2:J19</xm:sqref>
+          <xm:sqref>J2:J23</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1394,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Excel clean names for weights
</commit_message>
<xml_diff>
--- a/Assets/Data/Weights.xlsx
+++ b/Assets/Data/Weights.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="56">
   <si>
     <t>Type</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>TrapezeW</t>
-  </si>
-  <si>
-    <t>Triangle NW</t>
   </si>
   <si>
     <t>ParallelogramSN</t>
@@ -1721,7 +1718,7 @@
   <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -1758,49 +1755,49 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>47</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>49</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>51</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>52</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>54</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:28">
@@ -1819,13 +1816,13 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
         <v>26</v>
@@ -1847,25 +1844,25 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
         <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J3" t="s">
         <v>26</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L3" t="s">
         <v>13</v>
@@ -1887,13 +1884,13 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -1915,13 +1912,13 @@
         <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -1943,19 +1940,19 @@
         <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
         <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J6" t="s">
         <v>34</v>
@@ -1977,28 +1974,28 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J7" t="s">
         <v>29</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -2017,31 +2014,31 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J8" t="s">
         <v>13</v>
       </c>
       <c r="K8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L8" t="s">
         <v>29</v>
       </c>
       <c r="M8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N8" t="s">
         <v>30</v>
@@ -2063,49 +2060,49 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
         <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
         <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J9" t="s">
         <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L9" t="s">
         <v>26</v>
       </c>
       <c r="M9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N9" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P9" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>55</v>
+      </c>
+      <c r="R9" t="s">
         <v>39</v>
       </c>
-      <c r="O9" t="s">
-        <v>56</v>
-      </c>
-      <c r="P9" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>56</v>
-      </c>
-      <c r="R9" t="s">
-        <v>40</v>
-      </c>
       <c r="S9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T9" t="s">
         <v>25</v>
@@ -2192,7 +2189,7 @@
     <row r="6" spans="1:2">
       <c r="A6" t="str">
         <f>Sequences!C7&amp;":"&amp;Sequences!D7&amp;Sequences!E7&amp;Sequences!F7&amp;Sequences!G7&amp;Sequences!H7&amp;Sequences!I7&amp;Sequences!J7&amp;Sequences!K7&amp;Sequences!L7&amp;Sequences!M7&amp;Sequences!N7&amp;Sequences!O7&amp;Sequences!P7&amp;Sequences!Q7&amp;Sequences!R7&amp;Sequences!S7&amp;Sequences!T7&amp;Sequences!U7&amp;Sequences!V7&amp;Sequences!W7&amp;Sequences!X7&amp;Sequences!Y7&amp;Sequences!Z7&amp;Sequences!AA7&amp;Sequences!AB7</f>
-        <v>Lvl2-2:TrapezeW:Triangle NW:Triangle NW:TriangleN:ParallelogramSN</v>
+        <v>Lvl2-2:TrapezeW:TriangleNW:TriangleNW:TriangleN:ParallelogramSN</v>
       </c>
       <c r="B6" t="str">
         <f>Sequences!C7&amp;":"&amp;Sequences!A7-1&amp;":"&amp;1</f>

</xml_diff>